<commit_message>
Enviando modificacoes na planilha
</commit_message>
<xml_diff>
--- a/Cobrancas.xlsx
+++ b/Cobrancas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Python\Desktop\Mentoria Sistema\Cobrancas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cursos\Estudos\Impressionador\ProjetoTK2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7374CE8-F490-4B29-B4BA-5039DFCA5F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B42B2-7250-41FC-AEA1-A101C63A763B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2838" yWindow="1536" windowWidth="17280" windowHeight="9438" xr2:uid="{035A09D7-5D5E-495B-98F5-7EC8A107D257}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{035A09D7-5D5E-495B-98F5-7EC8A107D257}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -425,17 +416,17 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.26171875" customWidth="1"/>
-    <col min="3" max="3" width="16.9453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,11 +440,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>5533988797979</v>
+      </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
@@ -461,11 +454,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>5533988797979</v>
+      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -473,11 +468,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>5533988797979</v>
+      </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -485,11 +482,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>5533988797979</v>
+      </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -497,11 +496,13 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>5533988797979</v>
+      </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>

</xml_diff>